<commit_message>
Update functionality for registru pacienti
</commit_message>
<xml_diff>
--- a/Registru_Pacienti/excel_database/Registru_pacienti.xlsx
+++ b/Registru_Pacienti/excel_database/Registru_pacienti.xlsx
@@ -9,7 +9,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="REGISTRU" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'REGISTRU'!$A$1:$V$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'REGISTRU'!$A$1:$V$5</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -454,7 +454,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V6"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,10 +466,10 @@
     <col width="21" customWidth="1" min="3" max="3"/>
     <col width="19" customWidth="1" min="4" max="4"/>
     <col width="23" customWidth="1" min="5" max="5"/>
-    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="21" customWidth="1" min="6" max="6"/>
     <col width="21" customWidth="1" min="7" max="7"/>
-    <col width="24" customWidth="1" min="8" max="8"/>
-    <col width="21" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="20" customWidth="1" min="9" max="9"/>
     <col width="19" customWidth="1" min="10" max="10"/>
     <col width="23" customWidth="1" min="11" max="11"/>
     <col width="25" customWidth="1" min="12" max="12"/>
@@ -481,7 +481,7 @@
     <col width="23" customWidth="1" min="18" max="18"/>
     <col width="23" customWidth="1" min="19" max="19"/>
     <col width="24" customWidth="1" min="20" max="20"/>
-    <col width="62" customWidth="1" min="21" max="21"/>
+    <col width="55" customWidth="1" min="21" max="21"/>
     <col width="164" customWidth="1" min="22" max="22"/>
   </cols>
   <sheetData>
@@ -925,17 +925,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>02-12-2023</t>
+          <t>13-12-2023</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>KILLIAN</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>MESSI</t>
+          <t>MBPAPPE</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -945,12 +945,12 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>911</t>
+          <t>07894125632</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>B-BUCURESTI</t>
+          <t>IF-ILFOV</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -960,7 +960,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Lege Speciala</t>
+          <t>Pensionar</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -968,9 +968,14 @@
           <t>YES</t>
         </is>
       </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>256312</t>
+        </is>
+      </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t xml:space="preserve">ASDADSA
+          <t xml:space="preserve">ASDSADSA
 </t>
         </is>
       </c>
@@ -1001,134 +1006,24 @@
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t xml:space="preserve">NON-APLICABIL
+          <t xml:space="preserve">EGOISM
 </t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t xml:space="preserve">A JUCA PANA LA 40 ANI
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>03-12-2023</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>VASILE</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>GHEORGHE</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>1623145566712</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>BUCOVINA</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>GURA HUMORULUI</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>SV-SUCEAVA</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>Pensionar</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>2336954</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PACIENT CU DIFICULTATI DE RESPIRATIE SI SOMN ANORMAL
-</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>OBSTRUCTIV</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>PILLOWS</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>1236</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>0.3MG/ML</t>
-        </is>
-      </c>
-      <c r="T6" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PARKINSON
-CANCER PROSTATIC
-DIABET ZAHARAT STADIU II
-</t>
-        </is>
-      </c>
-      <c r="V6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">XANAX SI MONITORIZARE LA SOMN PERMANENTA
+          <t xml:space="preserve">A SE MUTA LA REAL MADRID
 </t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V6"/>
+  <autoFilter ref="A1:V5"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Converting application to .exe app
</commit_message>
<xml_diff>
--- a/Registru_Pacienti/excel_database/Registru_pacienti.xlsx
+++ b/Registru_Pacienti/excel_database/Registru_pacienti.xlsx
@@ -9,7 +9,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="REGISTRU" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'REGISTRU'!$A$1:$V$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'REGISTRU'!$A$1:$V$6</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -454,7 +454,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,10 +466,10 @@
     <col width="21" customWidth="1" min="3" max="3"/>
     <col width="19" customWidth="1" min="4" max="4"/>
     <col width="23" customWidth="1" min="5" max="5"/>
-    <col width="21" customWidth="1" min="6" max="6"/>
+    <col width="22" customWidth="1" min="6" max="6"/>
     <col width="21" customWidth="1" min="7" max="7"/>
     <col width="20" customWidth="1" min="8" max="8"/>
-    <col width="20" customWidth="1" min="9" max="9"/>
+    <col width="21" customWidth="1" min="9" max="9"/>
     <col width="19" customWidth="1" min="10" max="10"/>
     <col width="23" customWidth="1" min="11" max="11"/>
     <col width="25" customWidth="1" min="12" max="12"/>
@@ -482,7 +482,7 @@
     <col width="23" customWidth="1" min="19" max="19"/>
     <col width="24" customWidth="1" min="20" max="20"/>
     <col width="55" customWidth="1" min="21" max="21"/>
-    <col width="164" customWidth="1" min="22" max="22"/>
+    <col width="200" customWidth="1" min="22" max="22"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -603,7 +603,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>01-12-2023</t>
+          <t>20-12-2023</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -709,10 +709,8 @@
       <c r="V2" t="inlineStr">
         <is>
           <t xml:space="preserve">A SE EVITA FRIGUL
-PARACETAMOL 2 X 3 ZILE
-SINGULAIR 1 X 7 ZILE
-VENTOLIN LA NEVOIE SI DIFICULTATI DE RESPIRATIE
-A SE REPETA CONTROLUL DUPA O LUNA DE ZILE.
+AERIUS LA NEVOIE
+A SE REPETA CONTROLUL DUPA 3 LUNI DE ZILE.
 </t>
         </is>
       </c>
@@ -827,27 +825,32 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>03-12-2023</t>
+          <t>13-12-2023</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>IOAN</t>
+          <t>KILLIAN</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>UNGUREANU</t>
+          <t>MBAPPEE</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1900106226805</t>
+          <t>1234567891011</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>078941256322</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>SV-SUCEAVA</t>
+          <t>IF-ILFOV</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -857,7 +860,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Salariat</t>
+          <t>Pensionar</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -867,13 +870,13 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t xml:space="preserve">CVBVCBVC </t>
+          <t>25631214</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t xml:space="preserve">VCBVCBVCBVCBVC
-</t>
+          <t>ASDSADSA
+ASDSADSADSADSASDGFDBGFDDSGDFGDFGDF</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
@@ -908,13 +911,20 @@
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t xml:space="preserve">DFXCCGBDFGFDGFD
-</t>
+          <t>EGOISM
+APLICATIA VAD CA FUNCTIONEAZA ACUMA</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t xml:space="preserve">FDGFDGFDGFDGFDGFD
+          <t xml:space="preserve">A SE MUTA LA REAL MADRID
+POATE RAMANE SI LA PSG DACA VREA SA FACA RECORDURI, DAR NU CRED CA E BUN
+ASASASA
+ASASASQ
+MAESTRO KIMBPEMBPE EEEEE
+ADADADADA
+ADASDASDSADSA
+TEST TEST TEST TEST SCROLL
 </t>
         </is>
       </c>
@@ -925,32 +935,42 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>13-12-2023</t>
+          <t>04-01-2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>KILLIAN</t>
+          <t>PUFOSEL</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>MBPAPPE</t>
+          <t>MOTAN</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1234567891011</t>
+          <t>1900106375492</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>07894125632</t>
+          <t>0748313438</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>PISICEASCA</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>BUCOVINA</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>IF-ILFOV</t>
+          <t>SV-SUCEAVA</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -960,7 +980,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Pensionar</t>
+          <t>Salariat</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -970,60 +990,170 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>256312</t>
+          <t>XDQWDX</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t xml:space="preserve">ASDSADSA
+          <t xml:space="preserve">PACIENT PISICOS, SE ADRESEAZA PENTRU RESPIRATOE ORALA NOCTURNA, ALINTATURI, MOTANELI.
 </t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>OBSTRUCTIV</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>NAZALA</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>BUNA</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>4-12</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">HIPODRAGANEALA
+</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">-CRESTE DRAGANEALA LA ZILNIC, 3 PUPURIX10/ZI, 20 IMBRATISARI/ZI, MINIM;
+-LA NEVOIE, SUPLIMENTERAZA DRAGANEALA.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>20-12-2023</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>GIGI</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>BECALI</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>1235558971414</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>078945632</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>PIPERA</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>B-BUCURESTI</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Lege Speciala</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>1213AAA</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PACIENT IN VARSTA DE 70 DE ANI SUFERA DE DEMENTA CHAMPIONS LEAGUE
+</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>NON-APLICABIL</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>NON-APLICABIL</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>NON-APLICABIL</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>NON-APLICABIL</t>
-        </is>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">EGOISM
-</t>
-        </is>
-      </c>
-      <c r="V5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">A SE MUTA LA REAL MADRID
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>NON-APLICABIL</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>NON-APLICABIL</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>NON-APLICABIL</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>NON-APLICABIL</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">OISM
+HAHALERISM
+</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A SE ASTEPTA PANA IN VARA ANULUI VIITOR CA POATE CASTIGA TITLUL. CONTROL IN IUNIE
 </t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V5"/>
+  <autoFilter ref="A1:V6"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Transfer to excel function for Programari
</commit_message>
<xml_diff>
--- a/Registru_Pacienti/excel_database/Registru_pacienti.xlsx
+++ b/Registru_Pacienti/excel_database/Registru_pacienti.xlsx
@@ -482,7 +482,7 @@
     <col width="23" customWidth="1" min="19" max="19"/>
     <col width="24" customWidth="1" min="20" max="20"/>
     <col width="55" customWidth="1" min="21" max="21"/>
-    <col width="200" customWidth="1" min="22" max="22"/>
+    <col width="176" customWidth="1" min="22" max="22"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -710,7 +710,7 @@
         <is>
           <t xml:space="preserve">A SE EVITA FRIGUL
 AERIUS LA NEVOIE
-A SE REPETA CONTROLUL DUPA 3 LUNI DE ZILE.
+A SE REPETA CONTROLUL DUPA 6 LUNI DE ZILE.
 </t>
         </is>
       </c>
@@ -922,8 +922,6 @@
 ASASASA
 ASASASQ
 MAESTRO KIMBPEMBPE EEEEE
-ADADADADA
-ADASDASDSADSA
 TEST TEST TEST TEST SCROLL
 </t>
         </is>

</xml_diff>

<commit_message>
Re-added registru_pacienti.exe after one drive fail
</commit_message>
<xml_diff>
--- a/Registru_Pacienti/excel_database/Registru_pacienti.xlsx
+++ b/Registru_Pacienti/excel_database/Registru_pacienti.xlsx
@@ -9,7 +9,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="REGISTRU" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'REGISTRU'!$A$1:$V$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'REGISTRU'!$A$1:$V$7</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -454,7 +454,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V6"/>
+  <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1150,8 +1150,121 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>03-01-2024</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>LEO</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>MESSI</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>1900106226823</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>5522333</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>INTER</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>MIMAI</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>STRAINATATE</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Salariat</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>256314</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">JUCATOR BUN
+</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>OBSTRUCTIV</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>PILLOWS</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>BUNA</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>0.325</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">TALENT PREA MARE
+</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A JUCA PANA LA CUPA MONDIALA SI A O CASTIGA
+</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:V6"/>
+  <autoFilter ref="A1:V7"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Excel writer tiny update
</commit_message>
<xml_diff>
--- a/Registru_Pacienti/excel_database/Registru_pacienti.xlsx
+++ b/Registru_Pacienti/excel_database/Registru_pacienti.xlsx
@@ -9,7 +9,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="REGISTRU" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'REGISTRU'!$A$1:$W$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'REGISTRU'!$A$1:$W$18</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -454,7 +454,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W17"/>
+  <dimension ref="A1:W18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,6 +483,7 @@
     <col width="24" customWidth="1" min="20" max="20"/>
     <col width="174" customWidth="1" min="21" max="21"/>
     <col width="101" customWidth="1" min="22" max="22"/>
+    <col width="14" customWidth="1" min="23" max="23"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -596,7 +597,7 @@
           <t>RECOMANDARE</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="W1" s="3" t="inlineStr">
         <is>
           <t>AHI</t>
         </is>
@@ -707,6 +708,11 @@
 </t>
         </is>
       </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -2142,8 +2148,111 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>16-01-2025</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>DXFDS</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>SDFDSFDS</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>1900106226805</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>OT-OLT</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Elev/Student</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>2368</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>NON-APLICABIL</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>NON-APLICABIL</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>NON-APLICABIL</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>NON-APLICABIL</t>
+        </is>
+      </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NON-APLICABIL
+</t>
+        </is>
+      </c>
+      <c r="V18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SDFDSFDSFDSFDS
+</t>
+        </is>
+      </c>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>9999</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:W17"/>
+  <autoFilter ref="A1:W18"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>